<commit_message>
Update script to accomodate phone number in south sudan upate script
</commit_message>
<xml_diff>
--- a/tests/unit/one_time_scripts/files/update_script_sudan.xlsx
+++ b/tests/unit/one_time_scripts/files/update_script_sudan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">unicef_id</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">birth_certificate_country_i_c</t>
   </si>
   <si>
+    <t xml:space="preserve">pp_phone_no_i_c</t>
+  </si>
+  <si>
     <t xml:space="preserve">IND-0</t>
   </si>
   <si>
@@ -131,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">Poland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+48603499023</t>
   </si>
   <si>
     <t xml:space="preserve">IND-1</t>
@@ -150,7 +156,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -179,6 +185,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -236,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,7 +261,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,10 +290,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3:S3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V3" activeCellId="0" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -298,7 +314,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="27.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -362,80 +378,86 @@
       <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
+      <c r="A2" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2" s="5" t="n">
         <v>33560</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>32</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
+      <c r="V2" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
+      <c r="A3" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="4"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>

</xml_diff>